<commit_message>
Hash Map added for signup page test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Signup" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -28,6 +28,45 @@
   </si>
   <si>
     <t>dasun1@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Minuga</t>
+  </si>
+  <si>
+    <t>Lakvindu</t>
+  </si>
+  <si>
+    <t>Minuga@123</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>minuga@abf.com</t>
   </si>
 </sst>
 </file>
@@ -388,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -425,12 +464,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>2005</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>